<commit_message>
changes to chat, upload starter
</commit_message>
<xml_diff>
--- a/student_data test.xlsx
+++ b/student_data test.xlsx
@@ -24,22 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>first name</t>
-  </si>
-  <si>
-    <t>last name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reg_number  </t>
-  </si>
-  <si>
-    <t>profile pic</t>
-  </si>
-  <si>
-    <t>YoS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Peter</t>
   </si>
@@ -47,7 +32,55 @@
     <t>Kamau</t>
   </si>
   <si>
-    <t>C026-01-0675/2020</t>
+    <t>score</t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
+  <si>
+    <t>C026-01-1333/2023</t>
+  </si>
+  <si>
+    <t>CCS 1101</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>C026-01-1334/2023</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Chege</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C026-01-1335/2024</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Mwangi</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>unit_code</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>reg_number</t>
   </si>
 </sst>
 </file>
@@ -365,11 +398,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -380,35 +411,84 @@
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>1.1000000000000001</v>
+      <c r="E3">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
email notification while uploading results
</commit_message>
<xml_diff>
--- a/student_data test.xlsx
+++ b/student_data test.xlsx
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Kamau</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>score</t>
   </si>
@@ -38,49 +32,37 @@
     <t>grade</t>
   </si>
   <si>
-    <t>C026-01-1333/2023</t>
-  </si>
-  <si>
-    <t>CCS 1101</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>C026-01-1334/2023</t>
-  </si>
-  <si>
-    <t>Charles</t>
-  </si>
-  <si>
-    <t>Chege</t>
+    <t>unit_code</t>
+  </si>
+  <si>
+    <t>reg_number</t>
+  </si>
+  <si>
+    <t>C026-01-0675/2020</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clarence </t>
+  </si>
+  <si>
+    <t>Gatama</t>
+  </si>
+  <si>
+    <t>CCS4205</t>
   </si>
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>C026-01-1335/2024</t>
-  </si>
-  <si>
-    <t>Simon</t>
-  </si>
-  <si>
-    <t>Mwangi</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>unit_code</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>reg_number</t>
+    <t>CCS4204</t>
   </si>
 </sst>
 </file>
@@ -398,37 +380,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="2" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -436,24 +420,24 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2">
-        <v>45</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -462,33 +446,13 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>